<commit_message>
messing with sunroof conversions
</commit_message>
<xml_diff>
--- a/Original Data Files/Project Sunroof Conversions.xlsx
+++ b/Original Data Files/Project Sunroof Conversions.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psimr\Documents\GitHub\Data-Visualization-Final-Project\Original Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCB82C8-4BCC-4D57-95EF-505DD80BC310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4130DD-60E7-4518-AC3A-E1BA91BE6DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E64AF2D2-6252-4152-A475-B6DB50FF868C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="New Jersey Overall" sheetId="2" r:id="rId1"/>
+    <sheet name="Zip Code Avg." sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="34">
   <si>
     <t>region_name</t>
   </si>
@@ -83,9 +83,6 @@
     <t>cars annually</t>
   </si>
   <si>
-    <t>Capacity</t>
-  </si>
-  <si>
     <t>https://sunroof.withgoogle.com/assets/data-explorer-methodology.pdf</t>
   </si>
   <si>
@@ -100,11 +97,56 @@
   <si>
     <t>trees planted for 10 years</t>
   </si>
+  <si>
+    <t xml:space="preserve">A typical passenger car emits 4.73 metric tons of CO2 annually </t>
+  </si>
+  <si>
+    <t>FROM SUNROOF WEBSITE:</t>
+  </si>
+  <si>
+    <t>car annually / CO2 tons</t>
+  </si>
+  <si>
+    <t>CO2 tons / car annually</t>
+  </si>
+  <si>
+    <t>car annually / kW</t>
+  </si>
+  <si>
+    <t>CO2 tons / tree planted</t>
+  </si>
+  <si>
+    <t>tree planted / CO2 tons</t>
+  </si>
+  <si>
+    <t>tree planted / kw</t>
+  </si>
+  <si>
+    <t>CO2 tons / kW</t>
+  </si>
+  <si>
+    <t>A planted and grown tree sequesters 0.039 metric tons of CO2 in 10 years.</t>
+  </si>
+  <si>
+    <t>cars taken off the road annually</t>
+  </si>
+  <si>
+    <t>CO2 offset</t>
+  </si>
+  <si>
+    <t>total kW</t>
+  </si>
+  <si>
+    <t>total MW</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -150,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -195,11 +237,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -225,6 +293,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,11 +613,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C7F072-984B-41F4-8E9E-7AFD0FAA8CC0}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="16.36328125" customWidth="1"/>
+    <col min="7" max="13" width="11.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="15">
+        <v>29256076.75</v>
+      </c>
+      <c r="C2" s="15">
+        <v>21441823.973146901</v>
+      </c>
+      <c r="D2" s="19">
+        <f>B2*$J$2</f>
+        <v>4533155.1740268283</v>
+      </c>
+      <c r="E2" s="19">
+        <f>B2*$M$2</f>
+        <v>549790358.28581798</v>
+      </c>
+      <c r="G2" s="18">
+        <f>C2/B2</f>
+        <v>0.73290154918488515</v>
+      </c>
+      <c r="H2" s="16">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="I2" s="16">
+        <f>1/H2</f>
+        <v>0.21141649048625791</v>
+      </c>
+      <c r="J2" s="18">
+        <f>I2*G2</f>
+        <v>0.15494747340060996</v>
+      </c>
+      <c r="K2" s="16">
+        <v>3.9E-2</v>
+      </c>
+      <c r="L2" s="16">
+        <f>1/K2</f>
+        <v>25.641025641025642</v>
+      </c>
+      <c r="M2" s="18">
+        <f>L2*G2</f>
+        <v>18.792347414997057</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
+        <v>29300</v>
+      </c>
+      <c r="B7" s="15">
+        <f>A7*1000</f>
+        <v>29300000</v>
+      </c>
+      <c r="C7" s="15">
+        <v>21400000</v>
+      </c>
+      <c r="D7" s="15">
+        <v>4700000</v>
+      </c>
+      <c r="E7" s="15">
+        <v>357000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G8" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G9" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G10" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G12" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G13" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07B9FA8-C9C4-44F8-8B86-97B1E3682B8F}">
   <dimension ref="A1:P478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G478"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +816,7 @@
         <v>14</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>13</v>
@@ -589,13 +834,13 @@
         <v>12</v>
       </c>
       <c r="N1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -837,7 +1082,7 @@
         <v>1872872.0819817209</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -12569,32 +12814,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C7F072-984B-41F4-8E9E-7AFD0FAA8CC0}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
baseline dashboard code - works
</commit_message>
<xml_diff>
--- a/Original Data Files/Project Sunroof Conversions.xlsx
+++ b/Original Data Files/Project Sunroof Conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psimr\Documents\GitHub\Data-Visualization-Final-Project\Original Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B0A530-4EF8-43C8-B9F1-6CB8FB0FCF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EB81A5-B77D-4544-956E-2C76FB79D445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E64AF2D2-6252-4152-A475-B6DB50FF868C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E64AF2D2-6252-4152-A475-B6DB50FF868C}"/>
   </bookViews>
   <sheets>
     <sheet name="New Jersey Overall" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="37">
   <si>
     <t>region_name</t>
   </si>
@@ -98,9 +98,6 @@
     <t>trees planted for 10 years</t>
   </si>
   <si>
-    <t xml:space="preserve">A typical passenger car emits 4.73 metric tons of CO2 annually </t>
-  </si>
-  <si>
     <t>FROM SUNROOF WEBSITE:</t>
   </si>
   <si>
@@ -138,6 +135,18 @@
   </si>
   <si>
     <t>total MW</t>
+  </si>
+  <si>
+    <t>https://www.seia.org/initiatives/whats-megawatt</t>
+  </si>
+  <si>
+    <t>In NJ 1 MW of capacity can power on average about 160 houses.</t>
+  </si>
+  <si>
+    <t>A typical passenger car emits 4.73 metric tons of CO2 annually.</t>
+  </si>
+  <si>
+    <t>1 kw of solar energy saves 1.38 metrics tons of CO2 emissions.</t>
   </si>
 </sst>
 </file>
@@ -614,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C7F072-984B-41F4-8E9E-7AFD0FAA8CC0}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,37 +641,37 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -713,21 +722,21 @@
     <row r="3" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>19</v>
@@ -753,27 +762,37 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="G8" s="8" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="G9" s="8" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="G10" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G12" s="8" t="s">
-        <v>8</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G11" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="G13" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G14" s="8" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G15" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>